<commit_message>
Update OS Metrics Measurement Results - XLRP Longitudinal Study - IOVS 2023.xlsx
</commit_message>
<xml_diff>
--- a/OS Metrics Measurement Results - XLRP Longitudinal Study - IOVS 2023.xlsx
+++ b/OS Metrics Measurement Results - XLRP Longitudinal Study - IOVS 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yzwang/Documents/GitHub/RFSW_RP_DLM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F84AEAE-4F29-4149-9F9D-34CD321B2ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8E7842-D6A7-B440-AA72-2067C782DD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34740" yWindow="1240" windowWidth="32820" windowHeight="21100" xr2:uid="{61C3B8C2-83F9-AE48-87F1-12C060ACE3E3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{61C3B8C2-83F9-AE48-87F1-12C060ACE3E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Grading" sheetId="2" r:id="rId1"/>
@@ -286,7 +286,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -322,13 +322,6 @@
       <color theme="1"/>
       <name val="Symbol"/>
       <charset val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -546,20 +539,6 @@
     <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -590,6 +569,20 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -908,7 +901,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D364" sqref="D364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -941,36 +934,36 @@
       </c>
     </row>
     <row r="2" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="46"/>
-      <c r="K2" s="47" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40"/>
+      <c r="K2" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="49"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="43"/>
       <c r="S2" s="20"/>
-      <c r="T2" s="50" t="s">
+      <c r="T2" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="52"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="45"/>
+      <c r="W2" s="46"/>
       <c r="X2" s="25"/>
-      <c r="Y2" s="50" t="s">
+      <c r="Y2" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="52"/>
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="45"/>
+      <c r="AB2" s="46"/>
     </row>
     <row r="3" spans="1:28" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -31506,11 +31499,11 @@
         <f>MIN(M4:M345)</f>
         <v>0.10449962</v>
       </c>
-      <c r="O348" s="43">
+      <c r="O348" s="37">
         <f>MIN(O4:O345)</f>
         <v>0.2775956662426971</v>
       </c>
-      <c r="Q348" s="43">
+      <c r="Q348" s="37">
         <f>MIN(Q4:Q345)</f>
         <v>4.9823154314754053E-4</v>
       </c>
@@ -31532,11 +31525,11 @@
         <f>MAX(M4:M345)</f>
         <v>28.5766305</v>
       </c>
-      <c r="O349" s="43">
+      <c r="O349" s="37">
         <f>MAX(O4:O345)</f>
         <v>5.342432309929281</v>
       </c>
-      <c r="Q349" s="43">
+      <c r="Q349" s="37">
         <f>MAX(Q4:Q345)</f>
         <v>0.80047404527587451</v>
       </c>
@@ -31583,7 +31576,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="J349" sqref="J349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31607,19 +31600,19 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="45"/>
-      <c r="G2" s="46"/>
-      <c r="J2" s="47" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40"/>
+      <c r="J2" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="49"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="43"/>
     </row>
     <row r="3" spans="1:15" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -37165,48 +37158,48 @@
         <v>8.8990488476571399E-4</v>
       </c>
     </row>
-    <row r="129" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="37" t="s">
+    <row r="129" spans="1:15" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="B129" s="38">
+      <c r="B129" s="48">
         <v>20.314236935564278</v>
       </c>
-      <c r="C129" s="38" t="s">
+      <c r="C129" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D129" s="39">
+      <c r="D129" s="49">
         <v>0.25580000000000003</v>
       </c>
-      <c r="E129" s="40">
+      <c r="E129" s="50">
         <v>11.25374532572855</v>
       </c>
-      <c r="F129" s="39">
+      <c r="F129" s="49">
         <v>0.65618221500000007</v>
       </c>
-      <c r="G129" s="39">
+      <c r="G129" s="49">
         <v>7.5584418323851495E-3</v>
       </c>
-      <c r="H129" s="40">
+      <c r="H129" s="50">
         <v>1.89017824074062</v>
       </c>
-      <c r="I129" s="41"/>
-      <c r="J129" s="40">
+      <c r="I129" s="51"/>
+      <c r="J129" s="50">
         <v>12.1554583333333</v>
       </c>
-      <c r="K129" s="40">
+      <c r="K129" s="50">
         <v>0</v>
       </c>
-      <c r="L129" s="40">
+      <c r="L129" s="50">
         <v>3.0240000000000002E-3</v>
       </c>
-      <c r="M129" s="40">
+      <c r="M129" s="50">
         <v>5.23772164208828E-3</v>
       </c>
-      <c r="N129" s="39">
+      <c r="N129" s="49">
         <v>3.6758105999999898E-5</v>
       </c>
-      <c r="O129" s="39">
+      <c r="O129" s="49">
         <v>6.3666907182002299E-5</v>
       </c>
     </row>
@@ -46731,7 +46724,7 @@
         <f>MIN(L4:L345)</f>
         <v>1.62446666666667E-3</v>
       </c>
-      <c r="N348" s="43">
+      <c r="N348" s="37">
         <f>MIN(N4:N345)</f>
         <v>1.1390344756825401E-5</v>
       </c>
@@ -46753,7 +46746,7 @@
         <f>MAX(L4:L345)</f>
         <v>25.483688999999998</v>
       </c>
-      <c r="N349" s="43">
+      <c r="N349" s="37">
         <f>MAX(N4:N345)</f>
         <v>0.775664379927269</v>
       </c>

</xml_diff>